<commit_message>
update with tracking adn re-org
</commit_message>
<xml_diff>
--- a/00_class_schedule/class_schedule_xlsx.xlsx
+++ b/00_class_schedule/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/ds4humans/00_class_schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D453286F-FCA1-6F42-8023-5B1FABA86E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F990F-CA86-3747-96C8-DB322254858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="860" windowWidth="38300" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="700" windowWidth="38300" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -56,22 +56,10 @@
     <t>Proscriptive v. Descriptive Questions</t>
   </si>
   <si>
-    <t>Exploratory Questions</t>
-  </si>
-  <si>
     <t>Teams 1</t>
   </si>
   <si>
     <t>Teams 2</t>
-  </si>
-  <si>
-    <t>Passive Prediction Questions</t>
-  </si>
-  <si>
-    <t>Causal Questions</t>
-  </si>
-  <si>
-    <t>Causal Questions: Experiments</t>
   </si>
   <si>
     <t>**MIDTERM**</t>
@@ -107,16 +95,6 @@
   </si>
   <si>
     <t>- `Descriptive versus Prescriptive Questions &lt;https://ds4humans.com/30_questions/05_descriptive_v_prescriptive.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `EDA &lt;https://ds4humans.com/30_questions/07_eda.html&gt;`_
-- `Using Exploratory Questions &lt;https://ds4humans.com/30_questions/10_using_exploratory_questions.html&gt;`_
-- `Answering Exploratory Questions &lt;https://ds4humans.com/30_questions/15_answering_exploratory_questions.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Review Team Charter Assignment &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/MIDS%20Team%20Charter%20Assignment.docx&gt;`_
-- Edmondson, Teaming, Chpt 2 from "Cognitive Barriers to Teaming" (p. 82) to end of Chapter (on Canvas)
- Optional: `Fostering Psychological Safety Tips &lt;https://docs.google.com/document/d/1PsnDMS2emcPLgMLFAQCXZjO7C4j2hJ7znOq_g2Zkjgk/export?format=pdf&gt;`_</t>
   </si>
   <si>
     <t>- `Using Causal Questions &lt;https://ds4humans.com/30_questions/30_using_causal_questions.html&gt;`_
@@ -133,32 +111,6 @@
   - Read Chpt 4 in Cunningham from start (different presentation of potential outcomes)</t>
   </si>
   <si>
-    <t>Experiments: Internal Validity (In Practice):
-- Kohvani, Tang and Xu: Chpt 2 (End to End Example)
-- Kohavi, Tang and Xu: Chpt 3, "Threats to Internal Validity" (p. 42-47) 
-- Kohvani, Tang and Xu: Chpt 19 (A/A Testing)</t>
-  </si>
-  <si>
-    <t>Overall Evaluation Criteria: Kohavi, Tang, and Xu Chpt 7.
-Finishing Internal Validity: 
-- Different Randomizations: Kohavi, Tang and Xu Chpt 22
-Experiments: External Validity (In Practice):
-- Kohavi, Tang and Xu, Chpt 3, "Threats to External Validity" to end (p. 47-54)
-- Kohvai, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)</t>
-  </si>
-  <si>
-    <t>Review Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designing Experiments
-- Power Calculations: Georgiev, Chpt 4 (Canvas)
-- `Don't stop experiments early! &lt;endogenous_stopping.ipynb&gt;`_
-</t>
-  </si>
-  <si>
-    <t>Optional Class</t>
-  </si>
-  <si>
     <t>AB Testing Review</t>
   </si>
   <si>
@@ -170,12 +122,6 @@
   </si>
   <si>
     <t>- `Causal Beyond Experiments &lt;https://ds4humans.com/35_causal/40_causal_inference_beyond_ab_testing.html&gt;`_</t>
-  </si>
-  <si>
-    <t>Exploratory Questions Feedback</t>
-  </si>
-  <si>
-    <t>- Bring comments on other teams' report</t>
   </si>
   <si>
     <t>Interpretation of Results</t>
@@ -222,9 +168,6 @@
     <t>incomeineq</t>
   </si>
   <si>
-    <t>power</t>
-  </si>
-  <si>
     <t>abtest</t>
   </si>
   <si>
@@ -244,15 +187,6 @@
   </si>
   <si>
     <t>acme</t>
-  </si>
-  <si>
-    <t>Explor Assign</t>
-  </si>
-  <si>
-    <t>- `Internal v. External Validity &lt;https://ds4humans.com/30_questions/17_exploratory_questions_internal_external.html&gt;`_
-- `Writing Good Notebooks &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/writing_good_jupyter_notebooks.html&gt;`_
-- Start Team Project
-- `Writing to Stakeholders &lt;../40_in_practice/25_writing_to_stakeholders.md&gt;`_</t>
   </si>
   <si>
     <t>Tu Jan 14</t>
@@ -355,6 +289,98 @@
   <si>
     <t>- admissions
 - interp</t>
+  </si>
+  <si>
+    <t>Passive Prediction Questions: Purpose and Alignment</t>
+  </si>
+  <si>
+    <t>Passive Prediction Questions: Internal and External Validity</t>
+  </si>
+  <si>
+    <t>Passive Prediction Questions: Interpretability</t>
+  </si>
+  <si>
+    <t>Passive Prediction Questions: Loss Functions</t>
+  </si>
+  <si>
+    <t>Exploratory Questions: Purpose, Internal and External Validity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- `Writing Good Notebooks &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/writing_good_jupyter_notebooks.html&gt;`_
+- Start Team Project
+- `Writing to Stakeholders &lt;../40_in_practice/25_writing_to_stakeholders.md&gt;`_</t>
+  </si>
+  <si>
+    <t>- `EDA &lt;https://ds4humans.com/30_questions/07_eda.html&gt;`_
+- `Using Exploratory Questions &lt;https://ds4humans.com/30_questions/10_using_exploratory_questions.html&gt;`_
+- `Answering Exploratory Questions &lt;https://ds4humans.com/30_questions/15_answering_exploratory_questions.html&gt;`_
+- `Internal v. External Validity &lt;https://ds4humans.com/30_questions/17_exploratory_questions_internal_external.html&gt;`_</t>
+  </si>
+  <si>
+    <t>Capstone With Training Wheels Assignment</t>
+  </si>
+  <si>
+    <t>Giving Feedback</t>
+  </si>
+  <si>
+    <t>Feedback Exercise?</t>
+  </si>
+  <si>
+    <t>- Explor Assign
+- How to write to stakeholders</t>
+  </si>
+  <si>
+    <t>Causal Questions: Purpose</t>
+  </si>
+  <si>
+    <t>Causal Questions: Potential Outcomes</t>
+  </si>
+  <si>
+    <t>Causal Questions: Experiments in Practice, Internal Validity</t>
+  </si>
+  <si>
+    <t>Causal Questions: Experiments in Practice, External Validity</t>
+  </si>
+  <si>
+    <t>Causal Questions: Experiments in Practice, Design</t>
+  </si>
+  <si>
+    <t>Causal Questions: Experiments, Bayesian Analysis &amp; Decision Theory</t>
+  </si>
+  <si>
+    <t>Causal Questions: Experiments, Bayesian Analysis</t>
+  </si>
+  <si>
+    <t>power
+p-value preview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designing Experiments
+- Statistical Power and Sample Sizes: GHV Ch 16
+- `Don't stop experiments early! &lt;endogenous_stopping.ipynb&gt;`_
+</t>
+  </si>
+  <si>
+    <t>Overall Evaluation Criteria: KTX Chpt 7.
+Finishing Internal Validity: 
+- Different Randomizations: KTX Chpt 22
+Experiments: External Validity (In Practice):
+- KTX, Chpt 3, "Threats to External Validity" to end (p. 47-54)
+- Kohvai, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)</t>
+  </si>
+  <si>
+    <t>Experiments: Internal Validity (In Practice):
+- KTX: Chpt 2 (End to End Example)
+- KTX: Chpt 3, "Threats to Internal Validity" (p. 42-47) 
+- KTX: Chpt 19 (A/A Testing)</t>
+  </si>
+  <si>
+    <t>- `Review Team Charter Assignment &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/MIDS%20Team%20Charter%20Assignment.docx&gt;`_
+- Edmondson, Teaming, Chpt 2 from "Cognitive Barriers to Teaming" (p. 82) to end of Chapter (on Canvas)
+- Cross Cultural Intelligence
+- When and How to Escalate
+ Optional: `Fostering Psychological Safety Tips &lt;https://docs.google.com/document/d/1PsnDMS2emcPLgMLFAQCXZjO7C4j2hJ7znOq_g2Zkjgk/export?format=pdf&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -1211,19 +1237,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" customWidth="1"/>
     <col min="3" max="3" width="64.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1234,369 +1260,368 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="187" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="187" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
         <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="187" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="187" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
       <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>